<commit_message>
Se agrega maestro de marca, tipo de activo y equipo y mq
</commit_message>
<xml_diff>
--- a/static/xls/fincas_pma.tipo_activo.xlsx
+++ b/static/xls/fincas_pma.tipo_activo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alcon\Documents\GitHub\fincas_pma\static\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zevcon\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209B0272-83AD-4848-ADB7-76ED2D8D66AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-4800" windowWidth="30936" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,55 +24,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>        ]</t>
-  </si>
-  <si>
-    <t>        ('E','EQUIPOS MAQUINARIAS VEHICULOS-INDUSTRIAL'),</t>
-  </si>
-  <si>
-    <t>        ('H','HERRAMIENTAS'),</t>
-  </si>
-  <si>
-    <t>        ('V','VEHICULOS-TRANSPORTE'),</t>
-  </si>
-  <si>
-    <t>        ('T','TERRENOS Y BIENES NATURALES'),</t>
-  </si>
-  <si>
-    <t>        ('C','CONSTRUCCIONES'),</t>
-  </si>
-  <si>
-    <t>        ('I','INSTALACIONES TECNICAS'),</t>
-  </si>
-  <si>
-    <t>        ('M','MOBILIARIO'),</t>
-  </si>
-  <si>
-    <t>        ('B','EQUIPOS INFORMATICOS'),</t>
-  </si>
-  <si>
-    <t>        ('O','OTROS')</t>
-  </si>
-  <si>
-    <t>        F</t>
-  </si>
-  <si>
-    <t>,'MAQUINARIAS INDUSTRIALES FIJA'),</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>MAQUINARIAS INDUSTRIALES FIJA</t>
+  </si>
+  <si>
+    <t>EQUIPOS MAQUINARIAS VEHICULOS-INDUSTRIAL</t>
+  </si>
+  <si>
+    <t>HERRAMIENTAS</t>
+  </si>
+  <si>
+    <t>VEHICULOS-TRANSPORTE</t>
+  </si>
+  <si>
+    <t>TERRENOS Y BIENES NATURALES</t>
+  </si>
+  <si>
+    <t>CONSTRUCCIONES</t>
+  </si>
+  <si>
+    <t>INSTALACIONES TECNICAS</t>
+  </si>
+  <si>
+    <t>MOBILIARIO</t>
+  </si>
+  <si>
+    <t>EQUIPOS INFORMATICOS</t>
+  </si>
+  <si>
+    <t>OTROS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,30 +71,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,12 +92,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,7 +112,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -188,7 +157,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -223,7 +192,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -404,87 +373,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" style="2" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="34.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajustes en archivos csv y carga de maestros. Version funcional validada
</commit_message>
<xml_diff>
--- a/static/xls/fincas_pma.tipo_activo.xlsx
+++ b/static/xls/fincas_pma.tipo_activo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zevcon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zevcon\Documents\fincas_pma\static\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16330" windowHeight="4810"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -377,7 +377,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>